<commit_message>
update output imaging computation
</commit_message>
<xml_diff>
--- a/templates/dataplant/4COM05_Imaging.xlsx
+++ b/templates/dataplant/4COM05_Imaging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBA6916-CE89-4466-90EC-9B01A68089A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7A0939-2883-44F9-ACFE-2001857DEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COm05_Imaging" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="120">
   <si>
     <t>Source Name</t>
   </si>
@@ -486,13 +486,16 @@
   </si>
   <si>
     <t>Authors Role Term Source REF</t>
+  </si>
+  <si>
+    <t>Derived Data File</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,12 +510,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -673,7 +670,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -683,6 +679,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,7 +733,7 @@
     <tableColumn id="27" xr3:uid="{CC29CA63-97CB-4156-A678-5BFEFD6C852B}" name="Parameter [image data analysis software]"/>
     <tableColumn id="28" xr3:uid="{AFA8A6FA-E7B7-483E-AC92-43D7020267C8}" name="Term Source REF (NFDI4PSO:1000129)"/>
     <tableColumn id="29" xr3:uid="{F0FAF2FE-30EF-4E37-996E-14745048B6D4}" name="Term Accession Number (NFDI4PSO:1000129)"/>
-    <tableColumn id="30" xr3:uid="{A12E3209-0D3E-4D1C-8E13-97FF36332E22}" name="Data File Name"/>
+    <tableColumn id="2" xr3:uid="{DD8351A7-5B80-4AAA-995E-41B17CF7FE4F}" name="Derived Data File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1040,7 +1037,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="646" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="610" row="3">
@@ -1073,36 +1070,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="74.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="58.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="39.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="104.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="105.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -1182,7 +1181,7 @@
         <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -1258,6 +1257,7 @@
       <c r="Y2" t="s">
         <v>112</v>
       </c>
+      <c r="Z2" s="13"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1305,6 +1305,7 @@
       <c r="Y3" t="s">
         <v>110</v>
       </c>
+      <c r="Z3" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1318,15 +1319,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65203DB1-CEB6-485D-A318-69575AAEF935}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1533,8 +1533,8 @@
       <c r="A27" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1565,314 +1565,314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="12"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L8" s="12"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1902,314 +1902,314 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+      <c r="H4" s="11"/>
+      <c r="I4" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L4" s="12"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12" t="s">
+      <c r="H5" s="11"/>
+      <c r="I5" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L5" s="12"/>
+      <c r="L5" s="11"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12" t="s">
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L6" s="12"/>
+      <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L8" s="12"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L10" s="12"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replace nfdi4pso terms in imaging computation template
</commit_message>
<xml_diff>
--- a/templates/dataplant/4COM05_Imaging.xlsx
+++ b/templates/dataplant/4COM05_Imaging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\ARCs und SWATE\ersatz von nfdi4pso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7A0939-2883-44F9-ACFE-2001857DEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C9CCB6-76BB-4E51-8D69-63BBEEC7BF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COm05_Imaging" sheetId="1" r:id="rId1"/>
@@ -52,75 +52,75 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{BB9A3614-4B66-498A-9D4E-80CBD1DEBF6F}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The unique identifier of this template. It will be auto generated.
-Reply:
+Antwort:
     id=0708cd5a-f3b4-400c-a188-9c6ac477906c</t>
       </text>
     </comment>
     <comment ref="A2" authorId="1" shapeId="0" xr:uid="{14D124C2-C21B-4F90-9CEE-5688E5E3032B}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate template.</t>
       </text>
     </comment>
     <comment ref="A3" authorId="2" shapeId="0" xr:uid="{4EFA4FC2-2986-4050-B46C-067EEA9512F7}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The current version of this template in SemVer notation.</t>
       </text>
     </comment>
     <comment ref="A4" authorId="3" shapeId="0" xr:uid="{68392C6C-BC61-4B1C-90A8-BF8E815CD421}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The description of this template. Use few sentences for succinctness.</t>
       </text>
     </comment>
     <comment ref="A5" authorId="4" shapeId="0" xr:uid="{BFEC8312-FE81-400E-9914-1305D9062478}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the template associated organisation. "DataPLANT" will trigger the "DataPLANT" batch of honor for the template.</t>
       </text>
     </comment>
     <comment ref="A6" authorId="5" shapeId="0" xr:uid="{6F594AD2-62F5-4957-B101-97AA7B311240}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The name of the Swate annotation table in the workbook of the template's excel file.</t>
       </text>
     </comment>
     <comment ref="A7" authorId="6" shapeId="0" xr:uid="{E009AF25-7068-4509-B33B-7D9FBE5888D1}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all ERs (endpoint repositories) targeted with this template. ERs are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A11" authorId="7" shapeId="0" xr:uid="{041EBAA7-1430-400A-A631-1A9111AF26B5}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     A list of all tags associated with this template. Tags are realized as Terms: &lt;term ref here&gt;</t>
       </text>
     </comment>
     <comment ref="A15" authorId="8" shapeId="0" xr:uid="{69198A12-B0F2-4850-82A0-2DC573651D21}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
     The author(s) of this template.</t>
       </text>
     </comment>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="119">
   <si>
     <t>Source Name</t>
   </si>
@@ -137,75 +137,27 @@
     <t>Parameter [use of image]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000135)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000135)</t>
-  </si>
-  <si>
     <t>Parameter [image processing technique]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000134)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000134)</t>
-  </si>
-  <si>
     <t>Parameter [image processing software]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000128)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000128)</t>
-  </si>
-  <si>
     <t>Parameter [image processing software parameters]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000130)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000130)</t>
-  </si>
-  <si>
     <t>Parameter [feature extraction strategy]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000133)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000133)</t>
-  </si>
-  <si>
     <t>Parameter [feature extraction software]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000131)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000131)</t>
-  </si>
-  <si>
     <t>Parameter [data analysis]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000132)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000132)</t>
-  </si>
-  <si>
     <t>Parameter [image data analysis software]</t>
   </si>
   <si>
-    <t>Term Source REF (NFDI4PSO:1000129)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000129)</t>
-  </si>
-  <si>
     <t>Data File Name</t>
   </si>
   <si>
@@ -326,9 +278,6 @@
     <t>Review comments</t>
   </si>
   <si>
-    <t>NFDI4PSO</t>
-  </si>
-  <si>
     <t>o</t>
   </si>
   <si>
@@ -347,54 +296,6 @@
     <t>Protocol_data analysis_Protocol</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000135</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000135</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000134</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000134</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000128</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000128</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000130</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000130</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000133</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000133</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000131</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000131</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000132</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000132</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:1000129</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000129</t>
-  </si>
-  <si>
     <t>image acquistion and feature extraction protocol |HCS image acquistion and feature extraction protocol</t>
   </si>
   <si>
@@ -461,18 +362,6 @@
     <t>MATLAB</t>
   </si>
   <si>
-    <t>user-specific</t>
-  </si>
-  <si>
-    <t>CHEBI</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_8735</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
     <t>DataPLANT</t>
   </si>
   <si>
@@ -489,13 +378,121 @@
   </si>
   <si>
     <t>Derived Data File</t>
+  </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000135)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000135)</t>
+  </si>
+  <si>
+    <t>Term Source REF (ERO:0001788)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (ERO:0001788)</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000128)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000128)</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000130)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000130)</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000133)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000133)</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000131)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000131)</t>
+  </si>
+  <si>
+    <t>Term Source REF (SIO:001051)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (SIO:001051)</t>
+  </si>
+  <si>
+    <t>Term Source REF (DPBO:1000129)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (DPBO:1000129)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000129</t>
+  </si>
+  <si>
+    <t>DPBO:1000129</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/SIO_001051</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000133</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000130</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000128</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ERO_0001788</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000135</t>
+  </si>
+  <si>
+    <t>DPBO:1000135</t>
+  </si>
+  <si>
+    <t>ERO:0001788</t>
+  </si>
+  <si>
+    <t>DPBO:1000128</t>
+  </si>
+  <si>
+    <t>DPBO:1000130</t>
+  </si>
+  <si>
+    <t>DPBO:1000133</t>
+  </si>
+  <si>
+    <t>DPBO:1000131</t>
+  </si>
+  <si>
+    <t>SIO:001051</t>
+  </si>
+  <si>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>ERO</t>
+  </si>
+  <si>
+    <t>SIO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_1000131</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,6 +504,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFF5F5F5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -638,10 +643,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -680,11 +686,85 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -709,30 +789,30 @@
   <autoFilter ref="A1:Z3" xr:uid="{1B8D8D55-F305-4C7D-A489-1FD68A6D6086}"/>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{D4DC74F2-ABF8-408F-BF2D-D3EAA9385BAC}" name="Source Name"/>
-    <tableColumn id="3" xr3:uid="{BDFE028D-A80A-4348-B880-F88408F7D535}" name="Parameter [use of image]"/>
-    <tableColumn id="4" xr3:uid="{FB714D18-92E8-4B3B-A210-5845B74F0406}" name="Term Source REF (NFDI4PSO:1000135)"/>
-    <tableColumn id="5" xr3:uid="{3E2E869B-0299-408E-A920-141D4D477269}" name="Term Accession Number (NFDI4PSO:1000135)"/>
-    <tableColumn id="6" xr3:uid="{BCB6C1A9-F60E-4647-8EA8-EC57F4EB8AFF}" name="Parameter [image processing technique]"/>
-    <tableColumn id="7" xr3:uid="{FCD6B9FC-CA76-4985-8BB5-A2F0EE26C7E2}" name="Term Source REF (NFDI4PSO:1000134)"/>
-    <tableColumn id="8" xr3:uid="{CF21C5E1-2A9C-46A1-AA4F-A4024AF0211F}" name="Term Accession Number (NFDI4PSO:1000134)"/>
-    <tableColumn id="9" xr3:uid="{B55F7D8C-0F52-4AA3-A049-6E7CDFC44D2E}" name="Parameter [image processing software]"/>
-    <tableColumn id="10" xr3:uid="{427AD50F-8358-4451-AA7B-FF7B7DCB3852}" name="Term Source REF (NFDI4PSO:1000128)"/>
-    <tableColumn id="11" xr3:uid="{8FE1F07A-A5E6-4386-BADE-637BDE23885A}" name="Term Accession Number (NFDI4PSO:1000128)"/>
-    <tableColumn id="12" xr3:uid="{95102D52-BDB1-482B-8843-5F47D4AEC9E1}" name="Parameter [image processing software parameters]"/>
-    <tableColumn id="13" xr3:uid="{D1294CA2-6B64-4C42-A5C5-923EC780505B}" name="Term Source REF (NFDI4PSO:1000130)"/>
-    <tableColumn id="14" xr3:uid="{48A357CE-B2E6-49D4-A701-B000E7B669FE}" name="Term Accession Number (NFDI4PSO:1000130)"/>
-    <tableColumn id="15" xr3:uid="{2DDB63AA-A844-41AB-A7E5-0A267DF9D5D2}" name="Parameter [feature extraction strategy]"/>
-    <tableColumn id="16" xr3:uid="{66A6A76F-94AD-4867-A4A5-511208B869A9}" name="Term Source REF (NFDI4PSO:1000133)"/>
-    <tableColumn id="17" xr3:uid="{6417FFC1-B4BE-4B34-BFB8-6537665E99EE}" name="Term Accession Number (NFDI4PSO:1000133)"/>
-    <tableColumn id="18" xr3:uid="{C4F58B9E-A708-4A0F-8E59-BF7EEDD9076A}" name="Parameter [feature extraction software]"/>
-    <tableColumn id="19" xr3:uid="{268AF60B-FF03-4F28-8E07-1B0CE4BF7835}" name="Term Source REF (NFDI4PSO:1000131)"/>
-    <tableColumn id="20" xr3:uid="{A99A8BD7-D857-4C7D-B443-E62FC518A2AE}" name="Term Accession Number (NFDI4PSO:1000131)"/>
-    <tableColumn id="24" xr3:uid="{F2DE8B60-E9D2-485B-A137-D9E5921E08AC}" name="Parameter [data analysis]"/>
-    <tableColumn id="25" xr3:uid="{99627201-2C62-45C8-9050-AE59F773CB6C}" name="Term Source REF (NFDI4PSO:1000132)"/>
-    <tableColumn id="26" xr3:uid="{0716AC80-31F7-4DC3-8B3E-5A95B9AC7721}" name="Term Accession Number (NFDI4PSO:1000132)"/>
-    <tableColumn id="27" xr3:uid="{CC29CA63-97CB-4156-A678-5BFEFD6C852B}" name="Parameter [image data analysis software]"/>
-    <tableColumn id="28" xr3:uid="{AFA8A6FA-E7B7-483E-AC92-43D7020267C8}" name="Term Source REF (NFDI4PSO:1000129)"/>
-    <tableColumn id="29" xr3:uid="{F0FAF2FE-30EF-4E37-996E-14745048B6D4}" name="Term Accession Number (NFDI4PSO:1000129)"/>
+    <tableColumn id="3" xr3:uid="{E952BA40-66E8-48E3-9FCE-90895306A47D}" name="Parameter [use of image]"/>
+    <tableColumn id="4" xr3:uid="{2AA5B30B-A20D-4A6F-A2D0-3DD987357F3B}" name="Term Source REF (DPBO:1000135)" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{1C1ADA13-B951-4572-BFC0-00747F316339}" name="Term Accession Number (DPBO:1000135)" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{DFD59A25-21D9-4A22-BA59-9617EBCDE992}" name="Parameter [image processing technique]" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{DD060580-DCE9-4E90-9D71-41A86028A410}" name="Term Source REF (ERO:0001788)" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{11414562-8833-449A-963C-5D703292EF8B}" name="Term Accession Number (ERO:0001788)" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{572320DE-94E1-4332-A0B2-E63DC8760468}" name="Parameter [image processing software]" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{00C3122A-BF92-4605-92CE-B895A4906116}" name="Term Source REF (DPBO:1000128)" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{7B33628D-C83F-4F40-A507-DEE8293F6AF2}" name="Term Accession Number (DPBO:1000128)" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{C44D644B-4D01-4E07-AB0F-8E33ACAE548C}" name="Parameter [image processing software parameters]" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{F7AA17C1-7F9E-458A-87AC-403E1B530976}" name="Term Source REF (DPBO:1000130)" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{50ACEE79-2E0C-4056-BB12-974BAE69BA7A}" name="Term Accession Number (DPBO:1000130)" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{92C7346C-ECD6-4213-B8D3-344CDDDEC036}" name="Parameter [feature extraction strategy]" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{39716A25-D65E-490C-A600-F6B73A848D91}" name="Term Source REF (DPBO:1000133)" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{BD0DAC2B-371F-43A6-ADF2-C3BA74EA1C15}" name="Term Accession Number (DPBO:1000133)" dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{44821E0F-E4D2-49F8-BC15-448BB05A559E}" name="Parameter [feature extraction software]" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{11ACB9DE-3A0B-43E7-9828-0172186BC4CA}" name="Term Source REF (DPBO:1000131)" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{9700E63A-CD1D-48B7-B3B9-FCAB86D119EA}" name="Term Accession Number (DPBO:1000131)" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{454BA68A-0A12-4786-92E9-A3E90A110088}" name="Parameter [data analysis]" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{7B9AFA7C-E71A-4AAD-9223-BB677CDA967E}" name="Term Source REF (SIO:001051)" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{0F55F9AF-C885-4329-A0DD-B9DD00AAB1B0}" name="Term Accession Number (SIO:001051)" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{B669869E-F774-44AA-BC14-D531327278D6}" name="Parameter [image data analysis software]" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{626F3B21-F4E4-41FB-91D1-3976456943EE}" name="Term Source REF (DPBO:1000129)" dataDxfId="1"/>
+    <tableColumn id="26" xr3:uid="{5E98214C-E7EA-4C82-8840-000714F840AB}" name="Term Accession Number (DPBO:1000129)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{DD8351A7-5B80-4AAA-995E-41B17CF7FE4F}" name="Derived Data File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1037,7 +1117,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="610" row="3">
@@ -1070,41 +1150,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="74.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="105.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="36.77734375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="37" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.77734375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="35.21875" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="38.109375" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1112,198 +1192,225 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="R1" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="U1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
       <c r="X1" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="Z1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" t="s">
-        <v>110</v>
+        <v>64</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" t="s">
-        <v>110</v>
+        <v>66</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J2" t="s">
-        <v>110</v>
+        <v>68</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" t="s">
-        <v>110</v>
+        <v>70</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="N2" t="s">
-        <v>104</v>
-      </c>
-      <c r="O2" t="s">
-        <v>110</v>
-      </c>
-      <c r="P2" t="s">
-        <v>110</v>
+        <v>71</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="Q2" t="s">
-        <v>105</v>
-      </c>
-      <c r="R2" t="s">
-        <v>110</v>
-      </c>
-      <c r="S2" t="s">
-        <v>110</v>
+        <v>72</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="T2" t="s">
-        <v>106</v>
-      </c>
-      <c r="U2" t="s">
-        <v>110</v>
-      </c>
-      <c r="V2" t="s">
-        <v>110</v>
+        <v>73</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="W2" t="s">
-        <v>107</v>
-      </c>
-      <c r="X2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>112</v>
+        <v>74</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="Z2" s="13"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" t="s">
-        <v>110</v>
+        <v>67</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" t="s">
-        <v>110</v>
+        <v>69</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P3" t="s">
-        <v>110</v>
+        <v>75</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="W3" t="s">
-        <v>109</v>
-      </c>
-      <c r="X3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>110</v>
+        <v>76</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="Z3" s="13"/>
     </row>
@@ -1320,218 +1427,218 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -1546,63 +1653,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3092793-3D7E-4CD8-9813-0B2F44F4BA56}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1618,249 +1727,249 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>75</v>
+        <v>116</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>77</v>
+        <v>115</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>79</v>
+        <v>115</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>81</v>
+        <v>115</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>83</v>
+        <v>115</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>85</v>
+        <v>117</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>87</v>
+        <v>115</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -1875,6 +1984,16 @@
       <c r="L11" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{8CACD085-DD9E-45F9-A5E9-11A04F21840E}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{4037374C-8537-4343-B2A0-09538D93C4EF}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{DBE44229-2F17-4419-858C-616DA54B9A8D}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{4F1028F4-2601-4807-8DE9-56FF4B4E2972}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{21EC8A95-47DB-44D2-89C0-CC561C8762A0}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{550D5DB6-7DA2-4515-8F8A-3E7D7FFC0FFE}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{CD61E474-BA5E-40EA-8BF1-6A5284F16360}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{AA099AEA-7EFF-4643-BF17-557124D1AB81}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1883,63 +2002,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9638EC50-B2AA-476B-BD06-451AAE7CC64A}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="94.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="94.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1955,249 +2076,249 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>75</v>
+        <v>116</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>77</v>
+        <v>115</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>79</v>
+        <v>115</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>81</v>
+        <v>115</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>83</v>
+        <v>115</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L8" s="11"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>85</v>
+        <v>117</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>87</v>
+        <v>115</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="L10" s="11"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
@@ -2212,6 +2333,16 @@
       <c r="L11" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{DEC87DA3-556A-45DD-B721-386DEF7FDBF6}"/>
+    <hyperlink ref="D9" r:id="rId2" xr:uid="{E60F5E60-D09F-4B5F-ACD0-47D1421E0406}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{4FB6D95A-DCC4-4911-868B-E84CF8BD7EB0}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00037FA0-3E08-4BD2-AA7C-BEA3D3BA3026}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{85C400D8-F923-493C-BCA9-C59DDE02F000}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{F3B71D80-9D8E-4746-9859-0F4EBAD3A14A}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{15875DE2-C182-49C0-A42A-6D3CDC7F2C2B}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{E73659F4-A028-4E70-96CE-A9080DDA48D5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>